<commit_message>
DATABASE: finalized 'uncategorized' staging data for 'download' table
</commit_message>
<xml_diff>
--- a/resources/database/data/db_download - staging data.xlsx
+++ b/resources/database/data/db_download - staging data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
   <si>
     <t>id</t>
   </si>
@@ -51,6 +51,315 @@
   </si>
   <si>
     <t>watched</t>
+  </si>
+  <si>
+    <t>Uncategorized</t>
+  </si>
+  <si>
+    <t>Akane Iro Ni Somaru Saka</t>
+  </si>
+  <si>
+    <t>Chaos;Head</t>
+  </si>
+  <si>
+    <t>Ebiten: Kouritsu Ebi Sugawa Koukou Tenmonbu</t>
+  </si>
+  <si>
+    <t>Ef - A Tale Of Melodies</t>
+  </si>
+  <si>
+    <t>Ef - A Tale Of Memories</t>
+  </si>
+  <si>
+    <t>Guilty Crown Kiseki Reassortment</t>
+  </si>
+  <si>
+    <t>Inukami!</t>
+  </si>
+  <si>
+    <t>Kashimashi - Girl Meets Girl</t>
+  </si>
+  <si>
+    <t>Love Hina</t>
+  </si>
+  <si>
+    <t>Love Hina Again</t>
+  </si>
+  <si>
+    <t>Love Love</t>
+  </si>
+  <si>
+    <t>Lovedol - Lovely Idol</t>
+  </si>
+  <si>
+    <t>Magikano</t>
+  </si>
+  <si>
+    <t>Mahoromantic</t>
+  </si>
+  <si>
+    <t>Mahoromantic - Automatic Maiden</t>
+  </si>
+  <si>
+    <t>Mahoromantic 2</t>
+  </si>
+  <si>
+    <t>Mahoromantic 2 Motto Utsukushii Mono</t>
+  </si>
+  <si>
+    <t>Mahou Shoujo Madoka Magica</t>
+  </si>
+  <si>
+    <t>Natsume Yuujin Chou</t>
+  </si>
+  <si>
+    <t>Natsume Yuujinchou San</t>
+  </si>
+  <si>
+    <t>Phi Brain: Kami No Puzzle 2</t>
+  </si>
+  <si>
+    <t>Sasameki Koto</t>
+  </si>
+  <si>
+    <t>Sengoku Collection</t>
+  </si>
+  <si>
+    <t>Senhime Zesshou Symphogear</t>
+  </si>
+  <si>
+    <t>Softenni</t>
+  </si>
+  <si>
+    <t>Tonagura!</t>
+  </si>
+  <si>
+    <t>Yumeria</t>
+  </si>
+  <si>
+    <t>Happy Lesson 2002</t>
+  </si>
+  <si>
+    <t>Alison To Lilia</t>
+  </si>
+  <si>
+    <t>Angelic Layer</t>
+  </si>
+  <si>
+    <t>Aoi Sekai Chuushin De</t>
+  </si>
+  <si>
+    <t>Aria The Animation</t>
+  </si>
+  <si>
+    <t>Aria The Natural</t>
+  </si>
+  <si>
+    <t>Aria The Origination</t>
+  </si>
+  <si>
+    <t>Baby Princess</t>
+  </si>
+  <si>
+    <t>Baka To Test To Shoukanjuu - Matsuri (Ova)</t>
+  </si>
+  <si>
+    <t>Bungaku Shoujo</t>
+  </si>
+  <si>
+    <t>Dance In The Vampire Bound</t>
+  </si>
+  <si>
+    <t>Denpa Teki Na Kanojo</t>
+  </si>
+  <si>
+    <t>Fractale</t>
+  </si>
+  <si>
+    <t>Gakuen Alice</t>
+  </si>
+  <si>
+    <t>Gokujo Mecha Mote Iinco *Check</t>
+  </si>
+  <si>
+    <t>Gokujo, Gokurakuin Joshikou Ryou Monogari</t>
+  </si>
+  <si>
+    <t>Gunslinger Girl</t>
+  </si>
+  <si>
+    <t>Hetalia</t>
+  </si>
+  <si>
+    <t>Higurashi No Naku Koro Ni Kai</t>
+  </si>
+  <si>
+    <t>Hyakko</t>
+  </si>
+  <si>
+    <t>Ichiban Ushiro No Daimaou</t>
+  </si>
+  <si>
+    <t>Ichiban Ushiro No Daimaou Special - Mo Hitotsu Omake No Daimaou</t>
+  </si>
+  <si>
+    <t>Ikkitousen</t>
+  </si>
+  <si>
+    <t>Ikkitousen Xx</t>
+  </si>
+  <si>
+    <t>Itazura Na Kiss</t>
+  </si>
+  <si>
+    <t>Jigoku Shougo Mitsuganae</t>
+  </si>
+  <si>
+    <t>Jigoku Shoujo</t>
+  </si>
+  <si>
+    <t>Jinrui Wa Suitai Shimashita</t>
+  </si>
+  <si>
+    <t>Kamuki Ni Sora</t>
+  </si>
+  <si>
+    <t>Kimi To Boku</t>
+  </si>
+  <si>
+    <t>Kimi To Boku 2</t>
+  </si>
+  <si>
+    <t>Kimiaru</t>
+  </si>
+  <si>
+    <t>Kimikiss Prue Rouge</t>
+  </si>
+  <si>
+    <t>Kono Aozora Ni Yakusoku Wo</t>
+  </si>
+  <si>
+    <t>Kurenai</t>
+  </si>
+  <si>
+    <t>Kuromajo-San Ga Tōru!!</t>
+  </si>
+  <si>
+    <t>Kuroshitsuji</t>
+  </si>
+  <si>
+    <t>Kyou Kara Maou</t>
+  </si>
+  <si>
+    <t>Kyou No Go No Ni</t>
+  </si>
+  <si>
+    <t>Mokke</t>
+  </si>
+  <si>
+    <t>Morita-San Wa Mukuchi</t>
+  </si>
+  <si>
+    <t>Morita-San Wa Mukuchi 2</t>
+  </si>
+  <si>
+    <t>Mouretsu Pirates</t>
+  </si>
+  <si>
+    <t>Nabari No Ou</t>
+  </si>
+  <si>
+    <t>Pandora Hearts</t>
+  </si>
+  <si>
+    <t>Queen'S Blade Gyokuza O Tsugu Mono</t>
+  </si>
+  <si>
+    <t>Queen'S Blade Rurou No Senshi</t>
+  </si>
+  <si>
+    <t>Rental Magica</t>
+  </si>
+  <si>
+    <t>Senki Zesshou Symphogear</t>
+  </si>
+  <si>
+    <t>Shi</t>
+  </si>
+  <si>
+    <t>Shiki</t>
+  </si>
+  <si>
+    <t>Shinkyoku Soukai Polyphonica Crimson S</t>
+  </si>
+  <si>
+    <t>Sora No Manimani</t>
+  </si>
+  <si>
+    <t>Sora O Miageru Shoujo No Hitomi Ni Utsuru Sekai</t>
+  </si>
+  <si>
+    <t>Suteki Tantei Labyrinth</t>
+  </si>
+  <si>
+    <t>Sweet Blue Flowers</t>
+  </si>
+  <si>
+    <t>Taishou Yakyuu Musume</t>
+  </si>
+  <si>
+    <t>Tantei Opera Milky Holmes</t>
+  </si>
+  <si>
+    <t>Tantei Opera Milky Holmes Dai 2 Maku</t>
+  </si>
+  <si>
+    <t>Tears To Tiara</t>
+  </si>
+  <si>
+    <t>Telepathy Shoujo Ran</t>
+  </si>
+  <si>
+    <t>Tengen Toppa Gurren Lagann</t>
+  </si>
+  <si>
+    <t>The Sacred Blacksmith</t>
+  </si>
+  <si>
+    <t>Umi Monogatari Anata Ga Ite Kureta Koto</t>
+  </si>
+  <si>
+    <t>Usagi Drops</t>
+  </si>
+  <si>
+    <t>Wagaya No Oinari-Sama</t>
+  </si>
+  <si>
+    <t>Weiss Survive</t>
+  </si>
+  <si>
+    <t>Weiss Survive R</t>
+  </si>
+  <si>
+    <t>White Album</t>
+  </si>
+  <si>
+    <t>Yoku Wakaru Gendai Mahou</t>
+  </si>
+  <si>
+    <t>Yume-Iro Patissiere</t>
+  </si>
+  <si>
+    <t>Yume-Iro Patissiere Sp Professional</t>
+  </si>
+  <si>
+    <t>Yumekui Merry</t>
+  </si>
+  <si>
+    <t>Happy Lesson Advance</t>
+  </si>
+  <si>
+    <t>Natsume Yuujinchou Zoku</t>
   </si>
 </sst>
 </file>
@@ -402,13 +711,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -439,6 +752,18 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
       <c r="G3">
         <v>1</v>
       </c>
@@ -447,6 +772,18 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
       <c r="G4">
         <v>2</v>
       </c>
@@ -454,7 +791,1410 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>109</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>107</v>
+      </c>
+      <c r="B68" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>30</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>87</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>34</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>94</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>96</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>97</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>99</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>35</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>97</v>
+      </c>
+      <c r="B96" t="s">
+        <v>102</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>98</v>
+      </c>
+      <c r="B97" t="s">
+        <v>103</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>99</v>
+      </c>
+      <c r="B98" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>100</v>
+      </c>
+      <c r="B99" t="s">
+        <v>105</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>101</v>
+      </c>
+      <c r="B100" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>103</v>
+      </c>
+      <c r="B101" t="s">
+        <v>107</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>104</v>
+      </c>
+      <c r="B102" t="s">
+        <v>108</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>105</v>
+      </c>
+      <c r="B103" t="s">
+        <v>109</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>106</v>
+      </c>
+      <c r="B104" t="s">
+        <v>36</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A3:D104">
+    <sortCondition ref="B3:B104"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DATABASE: added 'Winter 2014' to 'Fall 2014' download list
</commit_message>
<xml_diff>
--- a/resources/database/data/db_download - staging data.xlsx
+++ b/resources/database/data/db_download - staging data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="333">
   <si>
     <t>id</t>
   </si>
@@ -407,6 +407,9 @@
     <t>Vivid Red Operation</t>
   </si>
   <si>
+    <t>Winter 2014</t>
+  </si>
+  <si>
     <t>Gj-bu Chutou-bu</t>
   </si>
   <si>
@@ -629,6 +632,9 @@
     <t>Spring 2013</t>
   </si>
   <si>
+    <t>Spring 2014</t>
+  </si>
+  <si>
     <t>Kyouka no Kanata</t>
   </si>
   <si>
@@ -717,6 +723,306 @@
   </si>
   <si>
     <t>Fall 2013</t>
+  </si>
+  <si>
+    <t>Nisekoi</t>
+  </si>
+  <si>
+    <t>Oneechan ga Kita</t>
+  </si>
+  <si>
+    <t>Mikakunin de Shinkōkei</t>
+  </si>
+  <si>
+    <t>Tonari no Seki-kun</t>
+  </si>
+  <si>
+    <t>D-Frag!</t>
+  </si>
+  <si>
+    <t>Maken Ki! Two</t>
+  </si>
+  <si>
+    <t>Nourin</t>
+  </si>
+  <si>
+    <t>Silver Spoon Season 2</t>
+  </si>
+  <si>
+    <t>Wake Up, Girls!</t>
+  </si>
+  <si>
+    <t>Pupipō!</t>
+  </si>
+  <si>
+    <t>Robot Girls Z</t>
+  </si>
+  <si>
+    <t>Sekai Seifuku: Bouryaku no Zvezda</t>
+  </si>
+  <si>
+    <t>Super Sonico The Animation</t>
+  </si>
+  <si>
+    <t>Wizard Barristers: Benmashi Cecil</t>
+  </si>
+  <si>
+    <t>Wooser's Hand-to-Mouth Life Season 2</t>
+  </si>
+  <si>
+    <t>[MOVIE] Tamako Market</t>
+  </si>
+  <si>
+    <t>Hitsugi no Chaika</t>
+  </si>
+  <si>
+    <t>No Game no Life</t>
+  </si>
+  <si>
+    <t>Ryuugajou nanana no Maizoukin</t>
+  </si>
+  <si>
+    <t>Selector Infected WIXOSS</t>
+  </si>
+  <si>
+    <t>Ishuukan Friends</t>
+  </si>
+  <si>
+    <t>Gokukoku no Brynhildr</t>
+  </si>
+  <si>
+    <t>[MOVIE] Harmoine</t>
+  </si>
+  <si>
+    <t>Soredemo Sekai wa Utsukushii</t>
+  </si>
+  <si>
+    <t>Mangaka-san to Assistant-san to</t>
+  </si>
+  <si>
+    <t>Mekaku City Actors</t>
+  </si>
+  <si>
+    <t>Love Live! 2nd Season</t>
+  </si>
+  <si>
+    <t>Date a Live II</t>
+  </si>
+  <si>
+    <t>Fairy Tail 2014</t>
+  </si>
+  <si>
+    <t>Kanojo ga Flag o Oraretara</t>
+  </si>
+  <si>
+    <t>Kin'iro no Corda: Blue Sky (La Corda S2)</t>
+  </si>
+  <si>
+    <t>Mahouka Koukou no Retousei</t>
+  </si>
+  <si>
+    <t>Sadon Desu</t>
+  </si>
+  <si>
+    <t>Soul Eater Not!</t>
+  </si>
+  <si>
+    <t>[MOVIE] Sora no Otoshimono Movie</t>
+  </si>
+  <si>
+    <t>Black Bullet</t>
+  </si>
+  <si>
+    <t>Kamigami no Asobi ~Ludere deorum~</t>
+  </si>
+  <si>
+    <t>Pretty Rhythm: Star Selection</t>
+  </si>
+  <si>
+    <t>Seikoku no Dragonar</t>
+  </si>
+  <si>
+    <t>Yama no Susume 2</t>
+  </si>
+  <si>
+    <t>Baby Steps</t>
+  </si>
+  <si>
+    <t>[MOVIE] Pretty Rhythm All Stars Selection Prism Show Best Ten Movie</t>
+  </si>
+  <si>
+    <t>Ao Haru Ride</t>
+  </si>
+  <si>
+    <t>Fuutsu no Joshikousei ga [Locodol] Yate Mita</t>
+  </si>
+  <si>
+    <t>Gekkan Shoujo Nozaki-kun</t>
+  </si>
+  <si>
+    <t>Himegoto</t>
+  </si>
+  <si>
+    <t>Tokyo Ghoul</t>
+  </si>
+  <si>
+    <t>Momo Kyun Sword</t>
+  </si>
+  <si>
+    <t>Glasslip</t>
+  </si>
+  <si>
+    <t>Jinsei</t>
+  </si>
+  <si>
+    <t>Rokujiuma no Shinryakusha</t>
+  </si>
+  <si>
+    <t>Hanamonogatari</t>
+  </si>
+  <si>
+    <t>Hanayamata</t>
+  </si>
+  <si>
+    <t>Majmoji Rurumo</t>
+  </si>
+  <si>
+    <t>Persona 4 The Golden Animation</t>
+  </si>
+  <si>
+    <t>Seirei Tsukai no Blade Dance</t>
+  </si>
+  <si>
+    <t>Sabagebu</t>
+  </si>
+  <si>
+    <t>Tokyo ESP</t>
+  </si>
+  <si>
+    <t>Ai Mai Mi - Mousou Catastrophe</t>
+  </si>
+  <si>
+    <t>Akame ga Kill</t>
+  </si>
+  <si>
+    <t>Amagi Brilliant Park</t>
+  </si>
+  <si>
+    <t>Selector Spread WIXOOSS</t>
+  </si>
+  <si>
+    <t>Sora no Method</t>
+  </si>
+  <si>
+    <t>Ore, Twintails ni Narimasu</t>
+  </si>
+  <si>
+    <t>Shirobako</t>
+  </si>
+  <si>
+    <t>Trinity Seven: 7-nin no</t>
+  </si>
+  <si>
+    <t>Gugure! Kokkuri-san</t>
+  </si>
+  <si>
+    <t>Ai Tenchi Muyo!</t>
+  </si>
+  <si>
+    <t>Bonjour Koiaji Patisserie</t>
+  </si>
+  <si>
+    <t>Daitoshokan no Hitsujikai</t>
+  </si>
+  <si>
+    <t>Girlfriend (Kari)</t>
+  </si>
+  <si>
+    <t>Ookami Shoujo to Kuro Ouji</t>
+  </si>
+  <si>
+    <t>Shigatsu wa Kimi ni Uso</t>
+  </si>
+  <si>
+    <t>Grisaia no Kajitsu</t>
+  </si>
+  <si>
+    <t>Hitsugi no Chaika: Avenging Battle</t>
+  </si>
+  <si>
+    <t>Inou-Battle wa Nichijou-kei no Naka de</t>
+  </si>
+  <si>
+    <t>Log Horizon 2nd Series</t>
+  </si>
+  <si>
+    <t>Nanatsu no Taizai</t>
+  </si>
+  <si>
+    <t>Sanzoku no Musume Ronja</t>
+  </si>
+  <si>
+    <t>Ushinawareta Mirai wo Motomete</t>
+  </si>
+  <si>
+    <t>Yuuki Yuuna wa Yuusha de Aru</t>
+  </si>
+  <si>
+    <t>Denki-Gai no Honya-san</t>
+  </si>
+  <si>
+    <t>Madan no Ou to Vanadis</t>
+  </si>
+  <si>
+    <t>Mahoutsukai</t>
+  </si>
+  <si>
+    <t>Summer 2014</t>
+  </si>
+  <si>
+    <t>Fall 2014</t>
+  </si>
+  <si>
+    <t>Chuunibyou demo Koi ga Shitai II</t>
+  </si>
+  <si>
+    <t>Saikin, Imōto no Yōsu ga Chotto Okaishiin Da Ga.</t>
+  </si>
+  <si>
+    <t>Witch Craft Works</t>
+  </si>
+  <si>
+    <t>Sakura Trick</t>
+  </si>
+  <si>
+    <t>Saki: Zenkoku-hen</t>
+  </si>
+  <si>
+    <t>Seitokai Yakuindomo 2</t>
+  </si>
+  <si>
+    <t>Inari, Konkon, Koi Iroha</t>
+  </si>
+  <si>
+    <t>Toaru Hikuushi e no Koiuta</t>
+  </si>
+  <si>
+    <t>Gochuumon wo Usagi Desu ka</t>
+  </si>
+  <si>
+    <t>WAIT FOR AnimeNOW BD 1080</t>
+  </si>
+  <si>
+    <t>Bokura wa Minna Kawaiisou</t>
+  </si>
+  <si>
+    <t>Aldnoah Zero</t>
+  </si>
+  <si>
+    <t>DOWNLOAD SEASON 1</t>
+  </si>
+  <si>
+    <t>Hamatora Season 2</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -3070,7 +3376,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C116">
         <v>2</v>
@@ -3087,7 +3393,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -3104,7 +3410,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -3121,7 +3427,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -3138,7 +3444,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -3155,7 +3461,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -3172,7 +3478,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -3189,7 +3495,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3206,7 +3512,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -3223,7 +3529,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -3240,7 +3546,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -3257,7 +3563,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -3274,7 +3580,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -3291,7 +3597,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -3308,7 +3614,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -3325,7 +3631,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -3342,7 +3648,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -3359,7 +3665,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -3376,7 +3682,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C134">
         <v>3</v>
@@ -3385,7 +3691,7 @@
         <v>3</v>
       </c>
       <c r="E134" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3393,7 +3699,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C135">
         <v>3</v>
@@ -3402,7 +3708,7 @@
         <v>3</v>
       </c>
       <c r="E135" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3410,7 +3716,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C136">
         <v>3</v>
@@ -3419,7 +3725,7 @@
         <v>3</v>
       </c>
       <c r="E136" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3427,7 +3733,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C137">
         <v>3</v>
@@ -3436,7 +3742,7 @@
         <v>2</v>
       </c>
       <c r="E137" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3444,7 +3750,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C138">
         <v>3</v>
@@ -3453,7 +3759,7 @@
         <v>2</v>
       </c>
       <c r="E138" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3461,7 +3767,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C139">
         <v>3</v>
@@ -3470,7 +3776,7 @@
         <v>2</v>
       </c>
       <c r="E139" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3478,7 +3784,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C140">
         <v>3</v>
@@ -3487,7 +3793,7 @@
         <v>2</v>
       </c>
       <c r="E140" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3495,7 +3801,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C141">
         <v>3</v>
@@ -3504,7 +3810,7 @@
         <v>2</v>
       </c>
       <c r="E141" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3512,7 +3818,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C142">
         <v>3</v>
@@ -3521,7 +3827,7 @@
         <v>2</v>
       </c>
       <c r="E142" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3529,7 +3835,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C143">
         <v>3</v>
@@ -3538,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="E143" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3546,7 +3852,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C144">
         <v>3</v>
@@ -3555,7 +3861,7 @@
         <v>3</v>
       </c>
       <c r="E144" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -3563,7 +3869,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C145">
         <v>3</v>
@@ -3572,7 +3878,7 @@
         <v>3</v>
       </c>
       <c r="E145" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -3580,7 +3886,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C146">
         <v>2</v>
@@ -3589,7 +3895,7 @@
         <v>1</v>
       </c>
       <c r="E146" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -3597,7 +3903,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -3606,7 +3912,7 @@
         <v>2</v>
       </c>
       <c r="E147" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -3614,7 +3920,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -3623,7 +3929,7 @@
         <v>2</v>
       </c>
       <c r="E148" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -3631,7 +3937,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3640,7 +3946,7 @@
         <v>2</v>
       </c>
       <c r="E149" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -3648,7 +3954,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -3657,7 +3963,7 @@
         <v>2</v>
       </c>
       <c r="E150" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -3665,7 +3971,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -3674,7 +3980,7 @@
         <v>2</v>
       </c>
       <c r="E151" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -3682,7 +3988,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -3691,7 +3997,7 @@
         <v>2</v>
       </c>
       <c r="E152" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -3699,7 +4005,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -3708,7 +4014,7 @@
         <v>2</v>
       </c>
       <c r="E153" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -3716,7 +4022,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -3725,7 +4031,7 @@
         <v>2</v>
       </c>
       <c r="E154" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -3733,7 +4039,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -3742,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="E155" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -3750,7 +4056,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C156">
         <v>3</v>
@@ -3759,7 +4065,7 @@
         <v>3</v>
       </c>
       <c r="E156" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -3767,7 +4073,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C157">
         <v>3</v>
@@ -3776,10 +4082,10 @@
         <v>3</v>
       </c>
       <c r="E157" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F157" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3787,19 +4093,19 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
+        <v>189</v>
+      </c>
+      <c r="C158">
+        <v>3</v>
+      </c>
+      <c r="D158">
+        <v>3</v>
+      </c>
+      <c r="E158" t="s">
+        <v>200</v>
+      </c>
+      <c r="F158" t="s">
         <v>188</v>
-      </c>
-      <c r="C158">
-        <v>3</v>
-      </c>
-      <c r="D158">
-        <v>3</v>
-      </c>
-      <c r="E158" t="s">
-        <v>199</v>
-      </c>
-      <c r="F158" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -3807,7 +4113,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C159">
         <v>3</v>
@@ -3816,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="E159" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3824,7 +4130,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C160">
         <v>3</v>
@@ -3833,7 +4139,7 @@
         <v>2</v>
       </c>
       <c r="E160" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3841,7 +4147,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C161">
         <v>3</v>
@@ -3850,7 +4156,7 @@
         <v>2</v>
       </c>
       <c r="E161" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -3858,7 +4164,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C162">
         <v>3</v>
@@ -3867,7 +4173,7 @@
         <v>2</v>
       </c>
       <c r="E162" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -3875,7 +4181,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C163">
         <v>3</v>
@@ -3884,7 +4190,7 @@
         <v>2</v>
       </c>
       <c r="E163" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -3892,7 +4198,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C164">
         <v>3</v>
@@ -3901,7 +4207,7 @@
         <v>2</v>
       </c>
       <c r="E164" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -3909,7 +4215,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C165">
         <v>3</v>
@@ -3918,7 +4224,7 @@
         <v>1</v>
       </c>
       <c r="E165" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -3926,7 +4232,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C166">
         <v>3</v>
@@ -3935,7 +4241,7 @@
         <v>2</v>
       </c>
       <c r="E166" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -3943,7 +4249,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C167">
         <v>3</v>
@@ -3952,7 +4258,7 @@
         <v>2</v>
       </c>
       <c r="E167" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -3960,7 +4266,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C168">
         <v>3</v>
@@ -3969,7 +4275,7 @@
         <v>2</v>
       </c>
       <c r="E168" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -3977,7 +4283,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -3986,7 +4292,7 @@
         <v>3</v>
       </c>
       <c r="E169" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -3994,7 +4300,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -4003,7 +4309,7 @@
         <v>2</v>
       </c>
       <c r="E170" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4011,19 +4317,19 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
+        <v>194</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>2</v>
+      </c>
+      <c r="E171" t="s">
+        <v>200</v>
+      </c>
+      <c r="F171" t="s">
         <v>193</v>
-      </c>
-      <c r="C171">
-        <v>1</v>
-      </c>
-      <c r="D171">
-        <v>2</v>
-      </c>
-      <c r="E171" t="s">
-        <v>199</v>
-      </c>
-      <c r="F171" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -4031,7 +4337,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -4040,7 +4346,7 @@
         <v>2</v>
       </c>
       <c r="E172" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4048,7 +4354,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -4057,7 +4363,7 @@
         <v>2</v>
       </c>
       <c r="E173" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4065,7 +4371,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C174">
         <v>1</v>
@@ -4074,7 +4380,7 @@
         <v>2</v>
       </c>
       <c r="E174" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -4082,7 +4388,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -4091,7 +4397,7 @@
         <v>2</v>
       </c>
       <c r="E175" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -4099,7 +4405,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -4108,7 +4414,7 @@
         <v>2</v>
       </c>
       <c r="E176" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -4116,7 +4422,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C177">
         <v>2</v>
@@ -4125,7 +4431,7 @@
         <v>2</v>
       </c>
       <c r="E177" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -4133,7 +4439,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -4142,7 +4448,7 @@
         <v>2</v>
       </c>
       <c r="E178" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -4150,7 +4456,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -4159,7 +4465,7 @@
         <v>2</v>
       </c>
       <c r="E179" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -4167,7 +4473,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -4176,10 +4482,10 @@
         <v>1</v>
       </c>
       <c r="E180" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F180" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -4187,19 +4493,19 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
+        <v>197</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181" t="s">
+        <v>200</v>
+      </c>
+      <c r="F181" t="s">
         <v>196</v>
-      </c>
-      <c r="C181">
-        <v>1</v>
-      </c>
-      <c r="D181">
-        <v>1</v>
-      </c>
-      <c r="E181" t="s">
-        <v>199</v>
-      </c>
-      <c r="F181" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -4207,7 +4513,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -4216,7 +4522,7 @@
         <v>1</v>
       </c>
       <c r="E182" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -4224,7 +4530,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C183">
         <v>3</v>
@@ -4233,7 +4539,7 @@
         <v>3</v>
       </c>
       <c r="E183" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -4241,7 +4547,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C184">
         <v>3</v>
@@ -4250,7 +4556,7 @@
         <v>3</v>
       </c>
       <c r="E184" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -4258,7 +4564,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C185">
         <v>3</v>
@@ -4267,7 +4573,7 @@
         <v>3</v>
       </c>
       <c r="E185" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -4275,7 +4581,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C186">
         <v>3</v>
@@ -4284,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="E186" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -4292,7 +4598,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C187">
         <v>3</v>
@@ -4301,7 +4607,7 @@
         <v>2</v>
       </c>
       <c r="E187" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -4309,7 +4615,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C188">
         <v>3</v>
@@ -4318,7 +4624,7 @@
         <v>2</v>
       </c>
       <c r="E188" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -4326,7 +4632,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C189">
         <v>3</v>
@@ -4335,7 +4641,7 @@
         <v>2</v>
       </c>
       <c r="E189" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -4343,7 +4649,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C190">
         <v>3</v>
@@ -4352,7 +4658,7 @@
         <v>2</v>
       </c>
       <c r="E190" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4360,7 +4666,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C191">
         <v>3</v>
@@ -4369,7 +4675,7 @@
         <v>2</v>
       </c>
       <c r="E191" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -4377,7 +4683,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C192">
         <v>3</v>
@@ -4386,7 +4692,7 @@
         <v>2</v>
       </c>
       <c r="E192" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -4394,7 +4700,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C193">
         <v>3</v>
@@ -4403,10 +4709,10 @@
         <v>3</v>
       </c>
       <c r="E193" t="s">
+        <v>232</v>
+      </c>
+      <c r="F193" t="s">
         <v>230</v>
-      </c>
-      <c r="F193" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -4414,7 +4720,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C194">
         <v>3</v>
@@ -4423,7 +4729,7 @@
         <v>2</v>
       </c>
       <c r="E194" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -4431,7 +4737,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C195">
         <v>2</v>
@@ -4440,7 +4746,7 @@
         <v>2</v>
       </c>
       <c r="E195" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -4448,7 +4754,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C196">
         <v>1</v>
@@ -4457,7 +4763,7 @@
         <v>2</v>
       </c>
       <c r="E196" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -4465,7 +4771,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -4474,7 +4780,7 @@
         <v>2</v>
       </c>
       <c r="E197" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -4482,7 +4788,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -4491,7 +4797,7 @@
         <v>2</v>
       </c>
       <c r="E198" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -4499,7 +4805,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -4508,7 +4814,7 @@
         <v>2</v>
       </c>
       <c r="E199" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -4516,7 +4822,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -4525,7 +4831,7 @@
         <v>2</v>
       </c>
       <c r="E200" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -4533,7 +4839,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -4542,7 +4848,7 @@
         <v>2</v>
       </c>
       <c r="E201" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -4550,7 +4856,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -4559,7 +4865,7 @@
         <v>2</v>
       </c>
       <c r="E202" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -4567,7 +4873,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C203">
         <v>3</v>
@@ -4576,7 +4882,7 @@
         <v>1</v>
       </c>
       <c r="E203" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -4584,7 +4890,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -4593,10 +4899,10 @@
         <v>2</v>
       </c>
       <c r="E204" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F204" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -4604,7 +4910,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -4613,10 +4919,10 @@
         <v>2</v>
       </c>
       <c r="E205" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F205" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -4624,7 +4930,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -4633,7 +4939,7 @@
         <v>2</v>
       </c>
       <c r="E206" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -4641,7 +4947,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -4650,7 +4956,7 @@
         <v>2</v>
       </c>
       <c r="E207" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -4658,7 +4964,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -4667,565 +4973,1735 @@
         <v>1</v>
       </c>
       <c r="E208" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>319</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+      <c r="D209">
+        <v>3</v>
+      </c>
+      <c r="E209" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>320</v>
+      </c>
+      <c r="C210">
+        <v>3</v>
+      </c>
+      <c r="D210">
+        <v>3</v>
+      </c>
+      <c r="E210" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>321</v>
+      </c>
+      <c r="C211">
+        <v>3</v>
+      </c>
+      <c r="D211">
+        <v>3</v>
+      </c>
+      <c r="E211" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>322</v>
+      </c>
+      <c r="C212">
+        <v>3</v>
+      </c>
+      <c r="D212">
+        <v>3</v>
+      </c>
+      <c r="E212" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>323</v>
+      </c>
+      <c r="C213">
+        <v>3</v>
+      </c>
+      <c r="D213">
+        <v>3</v>
+      </c>
+      <c r="E213" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>212</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>324</v>
+      </c>
+      <c r="C214">
+        <v>3</v>
+      </c>
+      <c r="D214">
+        <v>3</v>
+      </c>
+      <c r="E214" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>233</v>
+      </c>
+      <c r="C215">
+        <v>3</v>
+      </c>
+      <c r="D215">
+        <v>2</v>
+      </c>
+      <c r="E215" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>234</v>
+      </c>
+      <c r="C216">
+        <v>3</v>
+      </c>
+      <c r="D216">
+        <v>2</v>
+      </c>
+      <c r="E216" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>235</v>
+      </c>
+      <c r="C217">
+        <v>3</v>
+      </c>
+      <c r="D217">
+        <v>2</v>
+      </c>
+      <c r="E217" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>216</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>236</v>
+      </c>
+      <c r="C218">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <v>2</v>
+      </c>
+      <c r="E218" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>325</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+      <c r="D219">
+        <v>3</v>
+      </c>
+      <c r="E219" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>218</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>326</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+      <c r="D220">
+        <v>3</v>
+      </c>
+      <c r="E220" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>237</v>
+      </c>
+      <c r="C221">
+        <v>3</v>
+      </c>
+      <c r="D221">
+        <v>2</v>
+      </c>
+      <c r="E221" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>220</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
+        <v>238</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+      <c r="D222">
+        <v>2</v>
+      </c>
+      <c r="E222" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>239</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223">
+        <v>2</v>
+      </c>
+      <c r="E223" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>222</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>240</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+      <c r="D224">
+        <v>2</v>
+      </c>
+      <c r="E224" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>241</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225">
+        <v>2</v>
+      </c>
+      <c r="E225" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>224</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
+        <v>242</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+      <c r="D226">
+        <v>2</v>
+      </c>
+      <c r="E226" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>243</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227">
+        <v>2</v>
+      </c>
+      <c r="E227" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>226</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
+        <v>244</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+      <c r="D228">
+        <v>2</v>
+      </c>
+      <c r="E228" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>245</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229">
+        <v>2</v>
+      </c>
+      <c r="E229" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>228</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
+        <v>246</v>
+      </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+      <c r="D230">
+        <v>2</v>
+      </c>
+      <c r="E230" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
+        <v>247</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+      <c r="D231">
+        <v>2</v>
+      </c>
+      <c r="E231" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>230</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
+        <v>145</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232">
+        <v>2</v>
+      </c>
+      <c r="E232" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
+        <v>248</v>
+      </c>
+      <c r="C233">
+        <v>3</v>
+      </c>
+      <c r="D233">
+        <v>3</v>
+      </c>
+      <c r="E233" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>232</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>327</v>
+      </c>
+      <c r="C234">
+        <v>3</v>
+      </c>
+      <c r="D234">
+        <v>3</v>
+      </c>
+      <c r="E234" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>249</v>
+      </c>
+      <c r="C235">
+        <v>3</v>
+      </c>
+      <c r="D235">
+        <v>3</v>
+      </c>
+      <c r="E235" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>234</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
+        <v>250</v>
+      </c>
+      <c r="C236">
+        <v>3</v>
+      </c>
+      <c r="D236">
+        <v>3</v>
+      </c>
+      <c r="E236" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>251</v>
+      </c>
+      <c r="C237">
+        <v>3</v>
+      </c>
+      <c r="D237">
+        <v>3</v>
+      </c>
+      <c r="E237" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>236</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B238" t="s">
+        <v>252</v>
+      </c>
+      <c r="C238">
+        <v>3</v>
+      </c>
+      <c r="D238">
+        <v>3</v>
+      </c>
+      <c r="E238" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>253</v>
+      </c>
+      <c r="C239">
+        <v>3</v>
+      </c>
+      <c r="D239">
+        <v>2</v>
+      </c>
+      <c r="E239" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>238</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
+        <v>254</v>
+      </c>
+      <c r="C240">
+        <v>3</v>
+      </c>
+      <c r="D240">
+        <v>2</v>
+      </c>
+      <c r="E240" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>255</v>
+      </c>
+      <c r="C241">
+        <v>3</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+      <c r="E241" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>240</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>256</v>
+      </c>
+      <c r="C242">
+        <v>3</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+      <c r="E242" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>257</v>
+      </c>
+      <c r="C243">
+        <v>1</v>
+      </c>
+      <c r="D243">
+        <v>3</v>
+      </c>
+      <c r="E243" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>242</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>258</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+      <c r="D244">
+        <v>3</v>
+      </c>
+      <c r="E244" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>329</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245">
+        <v>3</v>
+      </c>
+      <c r="E245" t="s">
+        <v>202</v>
+      </c>
+      <c r="F245" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>244</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>259</v>
+      </c>
+      <c r="C246">
+        <v>1</v>
+      </c>
+      <c r="D246">
+        <v>3</v>
+      </c>
+      <c r="E246" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>245</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
+        <v>260</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+      <c r="D247">
+        <v>3</v>
+      </c>
+      <c r="E247" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>246</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B248" t="s">
+        <v>261</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248">
+        <v>3</v>
+      </c>
+      <c r="E248" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>247</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>262</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249">
+        <v>3</v>
+      </c>
+      <c r="E249" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>248</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B250" t="s">
+        <v>263</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250">
+        <v>3</v>
+      </c>
+      <c r="E250" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>249</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B251" t="s">
+        <v>264</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251">
+        <v>3</v>
+      </c>
+      <c r="E251" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>250</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
+        <v>265</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+      <c r="D252">
+        <v>3</v>
+      </c>
+      <c r="E252" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>251</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B253" t="s">
+        <v>266</v>
+      </c>
+      <c r="C253">
+        <v>1</v>
+      </c>
+      <c r="D253">
+        <v>3</v>
+      </c>
+      <c r="E253" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>252</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B254" t="s">
+        <v>267</v>
+      </c>
+      <c r="C254">
+        <v>1</v>
+      </c>
+      <c r="D254">
+        <v>3</v>
+      </c>
+      <c r="E254" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>253</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B255" t="s">
+        <v>268</v>
+      </c>
+      <c r="C255">
+        <v>1</v>
+      </c>
+      <c r="D255">
+        <v>2</v>
+      </c>
+      <c r="E255" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>254</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B256" t="s">
+        <v>269</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="D256">
+        <v>2</v>
+      </c>
+      <c r="E256" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>255</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B257" t="s">
+        <v>270</v>
+      </c>
+      <c r="C257">
+        <v>1</v>
+      </c>
+      <c r="D257">
+        <v>2</v>
+      </c>
+      <c r="E257" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>256</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
+        <v>271</v>
+      </c>
+      <c r="C258">
+        <v>1</v>
+      </c>
+      <c r="D258">
+        <v>2</v>
+      </c>
+      <c r="E258" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>257</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B259" t="s">
+        <v>272</v>
+      </c>
+      <c r="C259">
+        <v>1</v>
+      </c>
+      <c r="D259">
+        <v>2</v>
+      </c>
+      <c r="E259" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>258</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B260" t="s">
+        <v>273</v>
+      </c>
+      <c r="C260">
+        <v>1</v>
+      </c>
+      <c r="D260">
+        <v>1</v>
+      </c>
+      <c r="E260" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>259</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
+        <v>274</v>
+      </c>
+      <c r="C261">
+        <v>1</v>
+      </c>
+      <c r="D261">
+        <v>1</v>
+      </c>
+      <c r="E261" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>260</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
+        <v>275</v>
+      </c>
+      <c r="C262">
+        <v>3</v>
+      </c>
+      <c r="D262">
+        <v>3</v>
+      </c>
+      <c r="E262" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>261</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
+        <v>276</v>
+      </c>
+      <c r="C263">
+        <v>3</v>
+      </c>
+      <c r="D263">
+        <v>3</v>
+      </c>
+      <c r="E263" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>262</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B264" t="s">
+        <v>277</v>
+      </c>
+      <c r="C264">
+        <v>3</v>
+      </c>
+      <c r="D264">
+        <v>3</v>
+      </c>
+      <c r="E264" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>263</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B265" t="s">
+        <v>278</v>
+      </c>
+      <c r="C265">
+        <v>3</v>
+      </c>
+      <c r="D265">
+        <v>3</v>
+      </c>
+      <c r="E265" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>264</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B266" t="s">
+        <v>279</v>
+      </c>
+      <c r="C266">
+        <v>3</v>
+      </c>
+      <c r="D266">
+        <v>2</v>
+      </c>
+      <c r="E266" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>265</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
+        <v>330</v>
+      </c>
+      <c r="C267">
+        <v>3</v>
+      </c>
+      <c r="D267">
+        <v>1</v>
+      </c>
+      <c r="E267" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>266</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B268" t="s">
+        <v>280</v>
+      </c>
+      <c r="C268">
+        <v>3</v>
+      </c>
+      <c r="D268">
+        <v>2</v>
+      </c>
+      <c r="E268" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>267</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
+        <v>281</v>
+      </c>
+      <c r="C269">
+        <v>1</v>
+      </c>
+      <c r="D269">
+        <v>3</v>
+      </c>
+      <c r="E269" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>268</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B270" t="s">
+        <v>282</v>
+      </c>
+      <c r="C270">
+        <v>2</v>
+      </c>
+      <c r="D270">
+        <v>3</v>
+      </c>
+      <c r="E270" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>269</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B271" t="s">
+        <v>283</v>
+      </c>
+      <c r="C271">
+        <v>3</v>
+      </c>
+      <c r="D271">
+        <v>3</v>
+      </c>
+      <c r="E271" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>270</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B272" t="s">
+        <v>284</v>
+      </c>
+      <c r="C272">
+        <v>1</v>
+      </c>
+      <c r="D272">
+        <v>2</v>
+      </c>
+      <c r="E272" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>271</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B273" t="s">
+        <v>285</v>
+      </c>
+      <c r="C273">
+        <v>1</v>
+      </c>
+      <c r="D273">
+        <v>2</v>
+      </c>
+      <c r="E273" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>272</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
+        <v>286</v>
+      </c>
+      <c r="C274">
+        <v>1</v>
+      </c>
+      <c r="D274">
+        <v>2</v>
+      </c>
+      <c r="E274" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>273</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
+        <v>287</v>
+      </c>
+      <c r="C275">
+        <v>3</v>
+      </c>
+      <c r="D275">
+        <v>2</v>
+      </c>
+      <c r="E275" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>274</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B276" t="s">
+        <v>332</v>
+      </c>
+      <c r="C276">
+        <v>1</v>
+      </c>
+      <c r="D276">
+        <v>2</v>
+      </c>
+      <c r="E276" t="s">
+        <v>317</v>
+      </c>
+      <c r="F276" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>275</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
+        <v>288</v>
+      </c>
+      <c r="C277">
+        <v>1</v>
+      </c>
+      <c r="D277">
+        <v>2</v>
+      </c>
+      <c r="E277" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>276</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B278" t="s">
+        <v>289</v>
+      </c>
+      <c r="C278">
+        <v>1</v>
+      </c>
+      <c r="D278">
+        <v>2</v>
+      </c>
+      <c r="E278" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>277</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B279" t="s">
+        <v>290</v>
+      </c>
+      <c r="C279">
+        <v>1</v>
+      </c>
+      <c r="D279">
+        <v>2</v>
+      </c>
+      <c r="E279" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>278</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>291</v>
+      </c>
+      <c r="C280">
+        <v>1</v>
+      </c>
+      <c r="D280">
+        <v>2</v>
+      </c>
+      <c r="E280" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>279</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
+        <v>292</v>
+      </c>
+      <c r="C281">
+        <v>1</v>
+      </c>
+      <c r="D281">
+        <v>2</v>
+      </c>
+      <c r="E281" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>280</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B282" t="s">
+        <v>293</v>
+      </c>
+      <c r="C282">
+        <v>3</v>
+      </c>
+      <c r="D282">
+        <v>3</v>
+      </c>
+      <c r="E282" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>281</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
+        <v>294</v>
+      </c>
+      <c r="C283">
+        <v>3</v>
+      </c>
+      <c r="D283">
+        <v>3</v>
+      </c>
+      <c r="E283" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>282</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B284" t="s">
+        <v>295</v>
+      </c>
+      <c r="C284">
+        <v>3</v>
+      </c>
+      <c r="D284">
+        <v>3</v>
+      </c>
+      <c r="E284" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>283</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285" t="s">
+        <v>296</v>
+      </c>
+      <c r="C285">
+        <v>3</v>
+      </c>
+      <c r="D285">
+        <v>2</v>
+      </c>
+      <c r="E285" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>284</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
+        <v>297</v>
+      </c>
+      <c r="C286">
+        <v>3</v>
+      </c>
+      <c r="D286">
+        <v>2</v>
+      </c>
+      <c r="E286" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>285</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
+        <v>298</v>
+      </c>
+      <c r="C287">
+        <v>3</v>
+      </c>
+      <c r="D287">
+        <v>2</v>
+      </c>
+      <c r="E287" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>286</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B288" t="s">
+        <v>299</v>
+      </c>
+      <c r="C288">
+        <v>3</v>
+      </c>
+      <c r="D288">
+        <v>1</v>
+      </c>
+      <c r="E288" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>287</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289" t="s">
+        <v>300</v>
+      </c>
+      <c r="C289">
+        <v>1</v>
+      </c>
+      <c r="D289">
+        <v>3</v>
+      </c>
+      <c r="E289" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>288</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290" t="s">
+        <v>301</v>
+      </c>
+      <c r="C290">
+        <v>1</v>
+      </c>
+      <c r="D290">
+        <v>3</v>
+      </c>
+      <c r="E290" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>289</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291" t="s">
+        <v>302</v>
+      </c>
+      <c r="C291">
+        <v>1</v>
+      </c>
+      <c r="D291">
+        <v>3</v>
+      </c>
+      <c r="E291" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>290</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B292" t="s">
+        <v>303</v>
+      </c>
+      <c r="C292">
+        <v>1</v>
+      </c>
+      <c r="D292">
+        <v>3</v>
+      </c>
+      <c r="E292" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>291</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B293" t="s">
+        <v>304</v>
+      </c>
+      <c r="C293">
+        <v>1</v>
+      </c>
+      <c r="D293">
+        <v>3</v>
+      </c>
+      <c r="E293" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>292</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B294" t="s">
+        <v>305</v>
+      </c>
+      <c r="C294">
+        <v>3</v>
+      </c>
+      <c r="D294">
+        <v>3</v>
+      </c>
+      <c r="E294" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>293</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B295" t="s">
+        <v>306</v>
+      </c>
+      <c r="C295">
+        <v>1</v>
+      </c>
+      <c r="D295">
+        <v>2</v>
+      </c>
+      <c r="E295" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>294</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B296" t="s">
+        <v>307</v>
+      </c>
+      <c r="C296">
+        <v>3</v>
+      </c>
+      <c r="D296">
+        <v>2</v>
+      </c>
+      <c r="E296" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>295</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B297" t="s">
+        <v>308</v>
+      </c>
+      <c r="C297">
+        <v>1</v>
+      </c>
+      <c r="D297">
+        <v>2</v>
+      </c>
+      <c r="E297" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>296</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B298" t="s">
+        <v>309</v>
+      </c>
+      <c r="C298">
+        <v>1</v>
+      </c>
+      <c r="D298">
+        <v>2</v>
+      </c>
+      <c r="E298" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>297</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B299" t="s">
+        <v>310</v>
+      </c>
+      <c r="C299">
+        <v>3</v>
+      </c>
+      <c r="D299">
+        <v>2</v>
+      </c>
+      <c r="E299" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>298</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B300" t="s">
+        <v>311</v>
+      </c>
+      <c r="C300">
+        <v>1</v>
+      </c>
+      <c r="D300">
+        <v>2</v>
+      </c>
+      <c r="E300" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>299</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B301" t="s">
+        <v>312</v>
+      </c>
+      <c r="C301">
+        <v>1</v>
+      </c>
+      <c r="D301">
+        <v>2</v>
+      </c>
+      <c r="E301" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>300</v>
       </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B302" t="s">
+        <v>313</v>
+      </c>
+      <c r="C302">
+        <v>1</v>
+      </c>
+      <c r="D302">
+        <v>2</v>
+      </c>
+      <c r="E302" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>301</v>
       </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B303" t="s">
+        <v>314</v>
+      </c>
+      <c r="C303">
+        <v>1</v>
+      </c>
+      <c r="D303">
+        <v>1</v>
+      </c>
+      <c r="E303" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>302</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B304" t="s">
+        <v>315</v>
+      </c>
+      <c r="C304">
+        <v>1</v>
+      </c>
+      <c r="D304">
+        <v>1</v>
+      </c>
+      <c r="E304" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>303</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B305" t="s">
+        <v>316</v>
+      </c>
+      <c r="C305">
+        <v>1</v>
+      </c>
+      <c r="D305">
+        <v>1</v>
+      </c>
+      <c r="E305" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>304</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>305</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>306</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>307</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>308</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>309</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>310</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>311</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>312</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>313</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>314</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>315</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>316</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>317</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>318</v>
       </c>

</xml_diff>

<commit_message>
DATABASE: added 'Winter 2015' to 'Spring 2015' download list
</commit_message>
<xml_diff>
--- a/resources/database/data/db_download - staging data.xlsx
+++ b/resources/database/data/db_download - staging data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="382">
   <si>
     <t>id</t>
   </si>
@@ -410,6 +410,9 @@
     <t>Winter 2014</t>
   </si>
   <si>
+    <t>Winter 2015</t>
+  </si>
+  <si>
     <t>Gj-bu Chutou-bu</t>
   </si>
   <si>
@@ -1023,6 +1026,150 @@
   </si>
   <si>
     <t>Hamatora Season 2</t>
+  </si>
+  <si>
+    <t>Aldnoah Zero 2</t>
+  </si>
+  <si>
+    <t>Absolute Duo</t>
+  </si>
+  <si>
+    <t>Durarara!!x2 Shou</t>
+  </si>
+  <si>
+    <t>Isuca</t>
+  </si>
+  <si>
+    <t>Juuou Mujin no Fafnir</t>
+  </si>
+  <si>
+    <t>Kamisama Hajimemashita 2nd</t>
+  </si>
+  <si>
+    <t>Kantai Collection : Kan Colle</t>
+  </si>
+  <si>
+    <t>Koufuku Graffiti [SHAFT]</t>
+  </si>
+  <si>
+    <t>Saenai Heroine no Sodate-kata</t>
+  </si>
+  <si>
+    <t>THE iDOLM@STER : Cinderella Girls</t>
+  </si>
+  <si>
+    <t>Yuri Kuma Arashi</t>
+  </si>
+  <si>
+    <t>Hori-san to Miyamura-kun: Shingakki</t>
+  </si>
+  <si>
+    <t>Shimai Maou no Keiyakusha</t>
+  </si>
+  <si>
+    <t>Ansatsu Kyoushitsu</t>
+  </si>
+  <si>
+    <t>Junketsu no Maria</t>
+  </si>
+  <si>
+    <t>Rolling Girls</t>
+  </si>
+  <si>
+    <t>Seiken Tsukai no World Break</t>
+  </si>
+  <si>
+    <t>Tantei Opera Milky Holmes TD</t>
+  </si>
+  <si>
+    <t>Tokyo Ghoul VA</t>
+  </si>
+  <si>
+    <t>Nisekoi 2</t>
+  </si>
+  <si>
+    <t>Yamadakun to Nananin no Majo</t>
+  </si>
+  <si>
+    <t>Shokugeki no Souma</t>
+  </si>
+  <si>
+    <t>Dungeon ni Deai o Motomeru no wa Machigatteiru Darou ka?</t>
+  </si>
+  <si>
+    <t>Denpa Kyoushi</t>
+  </si>
+  <si>
+    <t>Etotama</t>
+  </si>
+  <si>
+    <t>Grisaia no Meikyuu</t>
+  </si>
+  <si>
+    <t>Hello!! Kiniro Mosaic</t>
+  </si>
+  <si>
+    <t>High School DxD BorN</t>
+  </si>
+  <si>
+    <t>Kyoukai no Rinne</t>
+  </si>
+  <si>
+    <t>Plastic Memories</t>
+  </si>
+  <si>
+    <t>Re-Kan!</t>
+  </si>
+  <si>
+    <t>Urawa no Usagi-chan</t>
+  </si>
+  <si>
+    <t>Yahari Ore no Seishun Love Comedy wa Machigatteiru. Zoku</t>
+  </si>
+  <si>
+    <t>Gintama (2015)</t>
+  </si>
+  <si>
+    <t>Mahou Shoujo Lyrical Nanoha ViVid</t>
+  </si>
+  <si>
+    <t>Ore Monogatari!!</t>
+  </si>
+  <si>
+    <t>Owari no Seraph</t>
+  </si>
+  <si>
+    <t>Danna ga Nani wo Itteiru ka Wakaranai Ken 2</t>
+  </si>
+  <si>
+    <t>Teekyuu 4</t>
+  </si>
+  <si>
+    <t>Kyoukai no Kanata Movie: I'll Be Here - Kako-hen</t>
+  </si>
+  <si>
+    <t>Kyoukai no Kanata Movie: I'll Be Here - Mirai-hen</t>
+  </si>
+  <si>
+    <t>Love Live! The School Idol Movie</t>
+  </si>
+  <si>
+    <t>Persona 3 the Movie 3: Falling Down</t>
+  </si>
+  <si>
+    <t>Tamayura: Sotsugyou Shashin Part 1 - Me: Kizashi</t>
+  </si>
+  <si>
+    <t>Fate/stay night: Unlimited Blade Works 2nd Season</t>
+  </si>
+  <si>
+    <t>Dog Days" (Season 3)</t>
+  </si>
+  <si>
+    <t>Hibike! Euphonium</t>
+  </si>
+  <si>
+    <t>Spring 2015</t>
   </si>
 </sst>
 </file>
@@ -1374,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I341"/>
+  <dimension ref="A1:I352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A328" workbookViewId="0">
+      <selection activeCell="C334" sqref="C334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,7 +1547,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -3376,7 +3523,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C116">
         <v>2</v>
@@ -3393,7 +3540,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -3410,7 +3557,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -3427,7 +3574,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -3444,7 +3591,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -3461,7 +3608,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -3478,7 +3625,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -3495,7 +3642,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3512,7 +3659,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -3529,7 +3676,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -3546,7 +3693,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -3563,7 +3710,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -3580,7 +3727,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -3597,7 +3744,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -3614,7 +3761,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -3631,7 +3778,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -3648,7 +3795,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -3665,7 +3812,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -3682,7 +3829,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C134">
         <v>3</v>
@@ -3691,7 +3838,7 @@
         <v>3</v>
       </c>
       <c r="E134" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,7 +3846,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C135">
         <v>3</v>
@@ -3708,7 +3855,7 @@
         <v>3</v>
       </c>
       <c r="E135" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3716,7 +3863,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C136">
         <v>3</v>
@@ -3725,7 +3872,7 @@
         <v>3</v>
       </c>
       <c r="E136" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3733,7 +3880,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C137">
         <v>3</v>
@@ -3742,7 +3889,7 @@
         <v>2</v>
       </c>
       <c r="E137" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3750,7 +3897,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C138">
         <v>3</v>
@@ -3759,7 +3906,7 @@
         <v>2</v>
       </c>
       <c r="E138" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3767,7 +3914,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C139">
         <v>3</v>
@@ -3776,7 +3923,7 @@
         <v>2</v>
       </c>
       <c r="E139" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3784,7 +3931,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C140">
         <v>3</v>
@@ -3793,7 +3940,7 @@
         <v>2</v>
       </c>
       <c r="E140" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3801,7 +3948,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C141">
         <v>3</v>
@@ -3810,7 +3957,7 @@
         <v>2</v>
       </c>
       <c r="E141" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,7 +3965,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C142">
         <v>3</v>
@@ -3827,7 +3974,7 @@
         <v>2</v>
       </c>
       <c r="E142" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3835,7 +3982,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C143">
         <v>3</v>
@@ -3844,7 +3991,7 @@
         <v>1</v>
       </c>
       <c r="E143" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3852,7 +3999,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C144">
         <v>3</v>
@@ -3861,7 +4008,7 @@
         <v>3</v>
       </c>
       <c r="E144" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -3869,7 +4016,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C145">
         <v>3</v>
@@ -3878,7 +4025,7 @@
         <v>3</v>
       </c>
       <c r="E145" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -3886,7 +4033,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C146">
         <v>2</v>
@@ -3895,7 +4042,7 @@
         <v>1</v>
       </c>
       <c r="E146" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -3903,7 +4050,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -3912,7 +4059,7 @@
         <v>2</v>
       </c>
       <c r="E147" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -3920,7 +4067,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -3929,7 +4076,7 @@
         <v>2</v>
       </c>
       <c r="E148" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -3937,7 +4084,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -3946,7 +4093,7 @@
         <v>2</v>
       </c>
       <c r="E149" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -3954,7 +4101,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -3963,7 +4110,7 @@
         <v>2</v>
       </c>
       <c r="E150" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -3971,7 +4118,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -3980,7 +4127,7 @@
         <v>2</v>
       </c>
       <c r="E151" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -3988,7 +4135,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -3997,7 +4144,7 @@
         <v>2</v>
       </c>
       <c r="E152" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -4005,7 +4152,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -4014,7 +4161,7 @@
         <v>2</v>
       </c>
       <c r="E153" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -4022,7 +4169,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -4031,7 +4178,7 @@
         <v>2</v>
       </c>
       <c r="E154" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -4039,7 +4186,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -4048,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="E155" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4056,7 +4203,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C156">
         <v>3</v>
@@ -4065,7 +4212,7 @@
         <v>3</v>
       </c>
       <c r="E156" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4073,7 +4220,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C157">
         <v>3</v>
@@ -4082,10 +4229,10 @@
         <v>3</v>
       </c>
       <c r="E157" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F157" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4093,19 +4240,19 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
+        <v>190</v>
+      </c>
+      <c r="C158">
+        <v>3</v>
+      </c>
+      <c r="D158">
+        <v>3</v>
+      </c>
+      <c r="E158" t="s">
+        <v>201</v>
+      </c>
+      <c r="F158" t="s">
         <v>189</v>
-      </c>
-      <c r="C158">
-        <v>3</v>
-      </c>
-      <c r="D158">
-        <v>3</v>
-      </c>
-      <c r="E158" t="s">
-        <v>200</v>
-      </c>
-      <c r="F158" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4113,7 +4260,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C159">
         <v>3</v>
@@ -4122,7 +4269,7 @@
         <v>3</v>
       </c>
       <c r="E159" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4130,7 +4277,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C160">
         <v>3</v>
@@ -4139,7 +4286,7 @@
         <v>2</v>
       </c>
       <c r="E160" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -4147,7 +4294,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C161">
         <v>3</v>
@@ -4156,7 +4303,7 @@
         <v>2</v>
       </c>
       <c r="E161" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -4164,7 +4311,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C162">
         <v>3</v>
@@ -4173,7 +4320,7 @@
         <v>2</v>
       </c>
       <c r="E162" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4181,7 +4328,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C163">
         <v>3</v>
@@ -4190,7 +4337,7 @@
         <v>2</v>
       </c>
       <c r="E163" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4198,7 +4345,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C164">
         <v>3</v>
@@ -4207,7 +4354,7 @@
         <v>2</v>
       </c>
       <c r="E164" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4215,7 +4362,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C165">
         <v>3</v>
@@ -4224,7 +4371,7 @@
         <v>1</v>
       </c>
       <c r="E165" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -4232,7 +4379,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C166">
         <v>3</v>
@@ -4241,7 +4388,7 @@
         <v>2</v>
       </c>
       <c r="E166" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4249,7 +4396,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C167">
         <v>3</v>
@@ -4258,7 +4405,7 @@
         <v>2</v>
       </c>
       <c r="E167" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -4266,7 +4413,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C168">
         <v>3</v>
@@ -4275,7 +4422,7 @@
         <v>2</v>
       </c>
       <c r="E168" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -4283,7 +4430,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -4292,7 +4439,7 @@
         <v>3</v>
       </c>
       <c r="E169" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -4300,7 +4447,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -4309,7 +4456,7 @@
         <v>2</v>
       </c>
       <c r="E170" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4317,19 +4464,19 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
+        <v>195</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>2</v>
+      </c>
+      <c r="E171" t="s">
+        <v>201</v>
+      </c>
+      <c r="F171" t="s">
         <v>194</v>
-      </c>
-      <c r="C171">
-        <v>1</v>
-      </c>
-      <c r="D171">
-        <v>2</v>
-      </c>
-      <c r="E171" t="s">
-        <v>200</v>
-      </c>
-      <c r="F171" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -4337,7 +4484,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -4346,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="E172" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4354,7 +4501,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -4363,7 +4510,7 @@
         <v>2</v>
       </c>
       <c r="E173" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4371,7 +4518,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C174">
         <v>1</v>
@@ -4380,7 +4527,7 @@
         <v>2</v>
       </c>
       <c r="E174" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -4388,7 +4535,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -4397,7 +4544,7 @@
         <v>2</v>
       </c>
       <c r="E175" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -4405,7 +4552,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -4414,7 +4561,7 @@
         <v>2</v>
       </c>
       <c r="E176" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -4422,7 +4569,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C177">
         <v>2</v>
@@ -4431,7 +4578,7 @@
         <v>2</v>
       </c>
       <c r="E177" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -4439,7 +4586,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -4448,7 +4595,7 @@
         <v>2</v>
       </c>
       <c r="E178" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -4456,7 +4603,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -4465,7 +4612,7 @@
         <v>2</v>
       </c>
       <c r="E179" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -4473,7 +4620,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -4482,10 +4629,10 @@
         <v>1</v>
       </c>
       <c r="E180" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F180" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -4493,19 +4640,19 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
+        <v>198</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>1</v>
+      </c>
+      <c r="E181" t="s">
+        <v>201</v>
+      </c>
+      <c r="F181" t="s">
         <v>197</v>
-      </c>
-      <c r="C181">
-        <v>1</v>
-      </c>
-      <c r="D181">
-        <v>1</v>
-      </c>
-      <c r="E181" t="s">
-        <v>200</v>
-      </c>
-      <c r="F181" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -4513,7 +4660,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -4522,7 +4669,7 @@
         <v>1</v>
       </c>
       <c r="E182" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -4530,7 +4677,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C183">
         <v>3</v>
@@ -4539,7 +4686,7 @@
         <v>3</v>
       </c>
       <c r="E183" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -4547,7 +4694,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C184">
         <v>3</v>
@@ -4556,7 +4703,7 @@
         <v>3</v>
       </c>
       <c r="E184" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -4564,7 +4711,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C185">
         <v>3</v>
@@ -4573,7 +4720,7 @@
         <v>3</v>
       </c>
       <c r="E185" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -4581,7 +4728,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C186">
         <v>3</v>
@@ -4590,7 +4737,7 @@
         <v>2</v>
       </c>
       <c r="E186" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -4598,7 +4745,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C187">
         <v>3</v>
@@ -4607,7 +4754,7 @@
         <v>2</v>
       </c>
       <c r="E187" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -4615,7 +4762,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C188">
         <v>3</v>
@@ -4624,7 +4771,7 @@
         <v>2</v>
       </c>
       <c r="E188" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -4632,7 +4779,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C189">
         <v>3</v>
@@ -4641,7 +4788,7 @@
         <v>2</v>
       </c>
       <c r="E189" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -4649,7 +4796,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C190">
         <v>3</v>
@@ -4658,7 +4805,7 @@
         <v>2</v>
       </c>
       <c r="E190" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4666,7 +4813,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C191">
         <v>3</v>
@@ -4675,7 +4822,7 @@
         <v>2</v>
       </c>
       <c r="E191" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -4683,7 +4830,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C192">
         <v>3</v>
@@ -4692,7 +4839,7 @@
         <v>2</v>
       </c>
       <c r="E192" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -4700,19 +4847,19 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
+        <v>232</v>
+      </c>
+      <c r="C193">
+        <v>3</v>
+      </c>
+      <c r="D193">
+        <v>3</v>
+      </c>
+      <c r="E193" t="s">
+        <v>233</v>
+      </c>
+      <c r="F193" t="s">
         <v>231</v>
-      </c>
-      <c r="C193">
-        <v>3</v>
-      </c>
-      <c r="D193">
-        <v>3</v>
-      </c>
-      <c r="E193" t="s">
-        <v>232</v>
-      </c>
-      <c r="F193" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -4720,7 +4867,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C194">
         <v>3</v>
@@ -4729,7 +4876,7 @@
         <v>2</v>
       </c>
       <c r="E194" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -4737,7 +4884,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C195">
         <v>2</v>
@@ -4746,7 +4893,7 @@
         <v>2</v>
       </c>
       <c r="E195" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -4754,7 +4901,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C196">
         <v>1</v>
@@ -4763,7 +4910,7 @@
         <v>2</v>
       </c>
       <c r="E196" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -4771,7 +4918,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -4780,7 +4927,7 @@
         <v>2</v>
       </c>
       <c r="E197" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -4788,7 +4935,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C198">
         <v>1</v>
@@ -4797,7 +4944,7 @@
         <v>2</v>
       </c>
       <c r="E198" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -4805,7 +4952,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C199">
         <v>1</v>
@@ -4814,7 +4961,7 @@
         <v>2</v>
       </c>
       <c r="E199" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -4822,7 +4969,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C200">
         <v>1</v>
@@ -4831,7 +4978,7 @@
         <v>2</v>
       </c>
       <c r="E200" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -4839,7 +4986,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -4848,7 +4995,7 @@
         <v>2</v>
       </c>
       <c r="E201" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -4856,7 +5003,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C202">
         <v>1</v>
@@ -4865,7 +5012,7 @@
         <v>2</v>
       </c>
       <c r="E202" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -4873,7 +5020,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C203">
         <v>3</v>
@@ -4882,7 +5029,7 @@
         <v>1</v>
       </c>
       <c r="E203" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -4890,7 +5037,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -4899,10 +5046,10 @@
         <v>2</v>
       </c>
       <c r="E204" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F204" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -4910,7 +5057,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C205">
         <v>1</v>
@@ -4919,10 +5066,10 @@
         <v>2</v>
       </c>
       <c r="E205" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F205" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -4930,7 +5077,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -4939,7 +5086,7 @@
         <v>2</v>
       </c>
       <c r="E206" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -4947,7 +5094,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -4956,7 +5103,7 @@
         <v>2</v>
       </c>
       <c r="E207" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -4964,7 +5111,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C208">
         <v>1</v>
@@ -4973,7 +5120,7 @@
         <v>1</v>
       </c>
       <c r="E208" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -4981,7 +5128,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C209">
         <v>3</v>
@@ -4998,7 +5145,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C210">
         <v>3</v>
@@ -5015,7 +5162,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C211">
         <v>3</v>
@@ -5032,7 +5179,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C212">
         <v>3</v>
@@ -5049,7 +5196,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C213">
         <v>3</v>
@@ -5066,7 +5213,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C214">
         <v>3</v>
@@ -5083,7 +5230,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C215">
         <v>3</v>
@@ -5100,7 +5247,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C216">
         <v>3</v>
@@ -5117,7 +5264,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C217">
         <v>3</v>
@@ -5134,7 +5281,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C218">
         <v>2</v>
@@ -5151,7 +5298,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -5168,7 +5315,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -5185,7 +5332,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C221">
         <v>3</v>
@@ -5202,7 +5349,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -5219,7 +5366,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -5236,7 +5383,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -5253,7 +5400,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -5270,7 +5417,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -5287,7 +5434,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -5304,7 +5451,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -5321,7 +5468,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -5338,7 +5485,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -5355,7 +5502,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C231">
         <v>1</v>
@@ -5372,7 +5519,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C232">
         <v>1</v>
@@ -5389,7 +5536,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C233">
         <v>3</v>
@@ -5398,7 +5545,7 @@
         <v>3</v>
       </c>
       <c r="E233" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -5406,7 +5553,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C234">
         <v>3</v>
@@ -5415,7 +5562,7 @@
         <v>3</v>
       </c>
       <c r="E234" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -5423,7 +5570,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C235">
         <v>3</v>
@@ -5432,7 +5579,7 @@
         <v>3</v>
       </c>
       <c r="E235" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -5440,7 +5587,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C236">
         <v>3</v>
@@ -5449,7 +5596,7 @@
         <v>3</v>
       </c>
       <c r="E236" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -5457,7 +5604,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C237">
         <v>3</v>
@@ -5466,7 +5613,7 @@
         <v>3</v>
       </c>
       <c r="E237" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -5474,7 +5621,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C238">
         <v>3</v>
@@ -5483,7 +5630,7 @@
         <v>3</v>
       </c>
       <c r="E238" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -5491,7 +5638,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C239">
         <v>3</v>
@@ -5500,7 +5647,7 @@
         <v>2</v>
       </c>
       <c r="E239" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -5508,7 +5655,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C240">
         <v>3</v>
@@ -5517,7 +5664,7 @@
         <v>2</v>
       </c>
       <c r="E240" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
@@ -5525,7 +5672,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C241">
         <v>3</v>
@@ -5534,7 +5681,7 @@
         <v>1</v>
       </c>
       <c r="E241" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
@@ -5542,7 +5689,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C242">
         <v>3</v>
@@ -5551,7 +5698,7 @@
         <v>1</v>
       </c>
       <c r="E242" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
@@ -5559,7 +5706,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -5568,7 +5715,7 @@
         <v>3</v>
       </c>
       <c r="E243" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
@@ -5576,7 +5723,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -5585,7 +5732,7 @@
         <v>3</v>
       </c>
       <c r="E244" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
@@ -5593,19 +5740,19 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
+        <v>330</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245">
+        <v>3</v>
+      </c>
+      <c r="E245" t="s">
+        <v>203</v>
+      </c>
+      <c r="F245" t="s">
         <v>329</v>
-      </c>
-      <c r="C245">
-        <v>1</v>
-      </c>
-      <c r="D245">
-        <v>3</v>
-      </c>
-      <c r="E245" t="s">
-        <v>202</v>
-      </c>
-      <c r="F245" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
@@ -5613,7 +5760,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -5622,7 +5769,7 @@
         <v>3</v>
       </c>
       <c r="E246" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -5630,7 +5777,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -5639,7 +5786,7 @@
         <v>3</v>
       </c>
       <c r="E247" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
@@ -5647,7 +5794,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -5656,7 +5803,7 @@
         <v>3</v>
       </c>
       <c r="E248" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
@@ -5664,7 +5811,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -5673,7 +5820,7 @@
         <v>3</v>
       </c>
       <c r="E249" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -5681,7 +5828,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -5690,7 +5837,7 @@
         <v>3</v>
       </c>
       <c r="E250" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
@@ -5698,7 +5845,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -5707,7 +5854,7 @@
         <v>3</v>
       </c>
       <c r="E251" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
@@ -5715,7 +5862,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -5724,7 +5871,7 @@
         <v>3</v>
       </c>
       <c r="E252" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
@@ -5732,7 +5879,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -5741,7 +5888,7 @@
         <v>3</v>
       </c>
       <c r="E253" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
@@ -5749,7 +5896,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C254">
         <v>1</v>
@@ -5758,7 +5905,7 @@
         <v>3</v>
       </c>
       <c r="E254" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
@@ -5766,7 +5913,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -5775,7 +5922,7 @@
         <v>2</v>
       </c>
       <c r="E255" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
@@ -5783,7 +5930,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -5792,7 +5939,7 @@
         <v>2</v>
       </c>
       <c r="E256" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -5800,7 +5947,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -5809,7 +5956,7 @@
         <v>2</v>
       </c>
       <c r="E257" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -5817,7 +5964,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -5826,7 +5973,7 @@
         <v>2</v>
       </c>
       <c r="E258" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -5834,7 +5981,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C259">
         <v>1</v>
@@ -5843,7 +5990,7 @@
         <v>2</v>
       </c>
       <c r="E259" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -5851,7 +5998,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C260">
         <v>1</v>
@@ -5860,7 +6007,7 @@
         <v>1</v>
       </c>
       <c r="E260" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -5868,7 +6015,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -5877,7 +6024,7 @@
         <v>1</v>
       </c>
       <c r="E261" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -5885,7 +6032,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C262">
         <v>3</v>
@@ -5894,7 +6041,7 @@
         <v>3</v>
       </c>
       <c r="E262" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -5902,7 +6049,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C263">
         <v>3</v>
@@ -5911,7 +6058,7 @@
         <v>3</v>
       </c>
       <c r="E263" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -5919,7 +6066,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C264">
         <v>3</v>
@@ -5928,7 +6075,7 @@
         <v>3</v>
       </c>
       <c r="E264" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -5936,7 +6083,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C265">
         <v>3</v>
@@ -5945,7 +6092,7 @@
         <v>3</v>
       </c>
       <c r="E265" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -5953,7 +6100,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C266">
         <v>3</v>
@@ -5962,7 +6109,7 @@
         <v>2</v>
       </c>
       <c r="E266" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -5970,7 +6117,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C267">
         <v>3</v>
@@ -5979,7 +6126,7 @@
         <v>1</v>
       </c>
       <c r="E267" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -5987,7 +6134,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C268">
         <v>3</v>
@@ -5996,7 +6143,7 @@
         <v>2</v>
       </c>
       <c r="E268" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -6004,7 +6151,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -6013,7 +6160,7 @@
         <v>3</v>
       </c>
       <c r="E269" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6021,7 +6168,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C270">
         <v>2</v>
@@ -6030,7 +6177,7 @@
         <v>3</v>
       </c>
       <c r="E270" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6038,7 +6185,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C271">
         <v>3</v>
@@ -6047,7 +6194,7 @@
         <v>3</v>
       </c>
       <c r="E271" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6055,7 +6202,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C272">
         <v>1</v>
@@ -6064,7 +6211,7 @@
         <v>2</v>
       </c>
       <c r="E272" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
@@ -6072,7 +6219,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C273">
         <v>1</v>
@@ -6081,7 +6228,7 @@
         <v>2</v>
       </c>
       <c r="E273" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
@@ -6089,7 +6236,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C274">
         <v>1</v>
@@ -6098,7 +6245,7 @@
         <v>2</v>
       </c>
       <c r="E274" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
@@ -6106,7 +6253,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C275">
         <v>3</v>
@@ -6115,7 +6262,7 @@
         <v>2</v>
       </c>
       <c r="E275" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
@@ -6123,19 +6270,19 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
+        <v>333</v>
+      </c>
+      <c r="C276">
+        <v>1</v>
+      </c>
+      <c r="D276">
+        <v>2</v>
+      </c>
+      <c r="E276" t="s">
+        <v>318</v>
+      </c>
+      <c r="F276" t="s">
         <v>332</v>
-      </c>
-      <c r="C276">
-        <v>1</v>
-      </c>
-      <c r="D276">
-        <v>2</v>
-      </c>
-      <c r="E276" t="s">
-        <v>317</v>
-      </c>
-      <c r="F276" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
@@ -6143,7 +6290,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C277">
         <v>1</v>
@@ -6152,7 +6299,7 @@
         <v>2</v>
       </c>
       <c r="E277" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
@@ -6160,7 +6307,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C278">
         <v>1</v>
@@ -6169,7 +6316,7 @@
         <v>2</v>
       </c>
       <c r="E278" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
@@ -6177,7 +6324,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C279">
         <v>1</v>
@@ -6186,7 +6333,7 @@
         <v>2</v>
       </c>
       <c r="E279" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
@@ -6194,7 +6341,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C280">
         <v>1</v>
@@ -6203,7 +6350,7 @@
         <v>2</v>
       </c>
       <c r="E280" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
@@ -6211,7 +6358,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C281">
         <v>1</v>
@@ -6220,7 +6367,7 @@
         <v>2</v>
       </c>
       <c r="E281" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
@@ -6228,7 +6375,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C282">
         <v>3</v>
@@ -6237,7 +6384,7 @@
         <v>3</v>
       </c>
       <c r="E282" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -6245,7 +6392,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C283">
         <v>3</v>
@@ -6254,7 +6401,7 @@
         <v>3</v>
       </c>
       <c r="E283" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
@@ -6262,7 +6409,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C284">
         <v>3</v>
@@ -6271,7 +6418,7 @@
         <v>3</v>
       </c>
       <c r="E284" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
@@ -6279,7 +6426,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C285">
         <v>3</v>
@@ -6288,7 +6435,7 @@
         <v>2</v>
       </c>
       <c r="E285" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
@@ -6296,7 +6443,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C286">
         <v>3</v>
@@ -6305,7 +6452,7 @@
         <v>2</v>
       </c>
       <c r="E286" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
@@ -6313,7 +6460,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C287">
         <v>3</v>
@@ -6322,7 +6469,7 @@
         <v>2</v>
       </c>
       <c r="E287" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
@@ -6330,7 +6477,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C288">
         <v>3</v>
@@ -6339,7 +6486,7 @@
         <v>1</v>
       </c>
       <c r="E288" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -6347,7 +6494,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -6356,7 +6503,7 @@
         <v>3</v>
       </c>
       <c r="E289" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -6364,7 +6511,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C290">
         <v>1</v>
@@ -6373,7 +6520,7 @@
         <v>3</v>
       </c>
       <c r="E290" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -6381,7 +6528,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C291">
         <v>1</v>
@@ -6390,7 +6537,7 @@
         <v>3</v>
       </c>
       <c r="E291" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -6398,7 +6545,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C292">
         <v>1</v>
@@ -6407,7 +6554,7 @@
         <v>3</v>
       </c>
       <c r="E292" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -6415,7 +6562,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C293">
         <v>1</v>
@@ -6424,7 +6571,7 @@
         <v>3</v>
       </c>
       <c r="E293" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -6432,7 +6579,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C294">
         <v>3</v>
@@ -6441,7 +6588,7 @@
         <v>3</v>
       </c>
       <c r="E294" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -6449,7 +6596,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C295">
         <v>1</v>
@@ -6458,7 +6605,7 @@
         <v>2</v>
       </c>
       <c r="E295" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -6466,7 +6613,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C296">
         <v>3</v>
@@ -6475,7 +6622,7 @@
         <v>2</v>
       </c>
       <c r="E296" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -6483,7 +6630,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C297">
         <v>1</v>
@@ -6492,7 +6639,7 @@
         <v>2</v>
       </c>
       <c r="E297" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -6500,7 +6647,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C298">
         <v>1</v>
@@ -6509,7 +6656,7 @@
         <v>2</v>
       </c>
       <c r="E298" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -6517,7 +6664,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C299">
         <v>3</v>
@@ -6526,7 +6673,7 @@
         <v>2</v>
       </c>
       <c r="E299" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -6534,7 +6681,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C300">
         <v>1</v>
@@ -6543,7 +6690,7 @@
         <v>2</v>
       </c>
       <c r="E300" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -6551,7 +6698,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C301">
         <v>1</v>
@@ -6560,7 +6707,7 @@
         <v>2</v>
       </c>
       <c r="E301" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -6568,7 +6715,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C302">
         <v>1</v>
@@ -6577,7 +6724,7 @@
         <v>2</v>
       </c>
       <c r="E302" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -6585,7 +6732,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C303">
         <v>1</v>
@@ -6594,7 +6741,7 @@
         <v>1</v>
       </c>
       <c r="E303" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -6602,7 +6749,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C304">
         <v>1</v>
@@ -6611,7 +6758,7 @@
         <v>1</v>
       </c>
       <c r="E304" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -6619,7 +6766,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C305">
         <v>1</v>
@@ -6628,187 +6775,806 @@
         <v>1</v>
       </c>
       <c r="E305" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>304</v>
       </c>
+      <c r="B306" t="s">
+        <v>334</v>
+      </c>
+      <c r="C306">
+        <v>3</v>
+      </c>
+      <c r="D306">
+        <v>1</v>
+      </c>
+      <c r="E306" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>305</v>
       </c>
+      <c r="B307" t="s">
+        <v>335</v>
+      </c>
+      <c r="C307">
+        <v>1</v>
+      </c>
+      <c r="D307">
+        <v>3</v>
+      </c>
+      <c r="E307" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>306</v>
       </c>
+      <c r="B308" t="s">
+        <v>379</v>
+      </c>
+      <c r="C308">
+        <v>1</v>
+      </c>
+      <c r="D308">
+        <v>3</v>
+      </c>
+      <c r="E308" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>307</v>
       </c>
+      <c r="B309" t="s">
+        <v>336</v>
+      </c>
+      <c r="C309">
+        <v>1</v>
+      </c>
+      <c r="D309">
+        <v>3</v>
+      </c>
+      <c r="E309" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>308</v>
       </c>
+      <c r="B310" t="s">
+        <v>337</v>
+      </c>
+      <c r="C310">
+        <v>1</v>
+      </c>
+      <c r="D310">
+        <v>3</v>
+      </c>
+      <c r="E310" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>309</v>
       </c>
+      <c r="B311" t="s">
+        <v>338</v>
+      </c>
+      <c r="C311">
+        <v>1</v>
+      </c>
+      <c r="D311">
+        <v>3</v>
+      </c>
+      <c r="E311" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>310</v>
       </c>
+      <c r="B312" t="s">
+        <v>339</v>
+      </c>
+      <c r="C312">
+        <v>1</v>
+      </c>
+      <c r="D312">
+        <v>3</v>
+      </c>
+      <c r="E312" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>311</v>
       </c>
+      <c r="B313" t="s">
+        <v>340</v>
+      </c>
+      <c r="C313">
+        <v>1</v>
+      </c>
+      <c r="D313">
+        <v>3</v>
+      </c>
+      <c r="E313" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>312</v>
       </c>
+      <c r="B314" t="s">
+        <v>341</v>
+      </c>
+      <c r="C314">
+        <v>1</v>
+      </c>
+      <c r="D314">
+        <v>3</v>
+      </c>
+      <c r="E314" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>313</v>
       </c>
+      <c r="B315" t="s">
+        <v>342</v>
+      </c>
+      <c r="C315">
+        <v>1</v>
+      </c>
+      <c r="D315">
+        <v>3</v>
+      </c>
+      <c r="E315" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>314</v>
       </c>
+      <c r="B316" t="s">
+        <v>343</v>
+      </c>
+      <c r="C316">
+        <v>1</v>
+      </c>
+      <c r="D316">
+        <v>3</v>
+      </c>
+      <c r="E316" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>315</v>
       </c>
+      <c r="B317" t="s">
+        <v>344</v>
+      </c>
+      <c r="C317">
+        <v>1</v>
+      </c>
+      <c r="D317">
+        <v>3</v>
+      </c>
+      <c r="E317" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>316</v>
       </c>
+      <c r="B318" t="s">
+        <v>345</v>
+      </c>
+      <c r="C318">
+        <v>1</v>
+      </c>
+      <c r="D318">
+        <v>2</v>
+      </c>
+      <c r="E318" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>317</v>
       </c>
+      <c r="B319" t="s">
+        <v>346</v>
+      </c>
+      <c r="C319">
+        <v>1</v>
+      </c>
+      <c r="D319">
+        <v>2</v>
+      </c>
+      <c r="E319" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>318</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B320" t="s">
+        <v>347</v>
+      </c>
+      <c r="C320">
+        <v>1</v>
+      </c>
+      <c r="D320">
+        <v>1</v>
+      </c>
+      <c r="E320" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>319</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B321" t="s">
+        <v>348</v>
+      </c>
+      <c r="C321">
+        <v>3</v>
+      </c>
+      <c r="D321">
+        <v>1</v>
+      </c>
+      <c r="E321" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>320</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B322" t="s">
+        <v>349</v>
+      </c>
+      <c r="C322">
+        <v>1</v>
+      </c>
+      <c r="D322">
+        <v>1</v>
+      </c>
+      <c r="E322" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>321</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B323" t="s">
+        <v>350</v>
+      </c>
+      <c r="C323">
+        <v>1</v>
+      </c>
+      <c r="D323">
+        <v>1</v>
+      </c>
+      <c r="E323" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>322</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B324" t="s">
+        <v>351</v>
+      </c>
+      <c r="C324">
+        <v>1</v>
+      </c>
+      <c r="D324">
+        <v>1</v>
+      </c>
+      <c r="E324" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>323</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B325" t="s">
+        <v>352</v>
+      </c>
+      <c r="C325">
+        <v>2</v>
+      </c>
+      <c r="D325">
+        <v>1</v>
+      </c>
+      <c r="E325" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>324</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B326" t="s">
+        <v>353</v>
+      </c>
+      <c r="C326">
+        <v>3</v>
+      </c>
+      <c r="D326">
+        <v>3</v>
+      </c>
+      <c r="E326" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>325</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>354</v>
+      </c>
+      <c r="C327">
+        <v>3</v>
+      </c>
+      <c r="D327">
+        <v>3</v>
+      </c>
+      <c r="E327" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>326</v>
       </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B328" t="s">
+        <v>355</v>
+      </c>
+      <c r="C328">
+        <v>3</v>
+      </c>
+      <c r="D328">
+        <v>2</v>
+      </c>
+      <c r="E328" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>327</v>
       </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B329" t="s">
+        <v>356</v>
+      </c>
+      <c r="C329">
+        <v>3</v>
+      </c>
+      <c r="D329">
+        <v>2</v>
+      </c>
+      <c r="E329" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>328</v>
       </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B330" t="s">
+        <v>357</v>
+      </c>
+      <c r="C330">
+        <v>1</v>
+      </c>
+      <c r="D330">
+        <v>3</v>
+      </c>
+      <c r="E330" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>329</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B331" t="s">
+        <v>358</v>
+      </c>
+      <c r="C331">
+        <v>1</v>
+      </c>
+      <c r="D331">
+        <v>3</v>
+      </c>
+      <c r="E331" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>330</v>
       </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B332" t="s">
+        <v>359</v>
+      </c>
+      <c r="C332">
+        <v>1</v>
+      </c>
+      <c r="D332">
+        <v>3</v>
+      </c>
+      <c r="E332" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>331</v>
       </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B333" t="s">
+        <v>360</v>
+      </c>
+      <c r="C333">
+        <v>1</v>
+      </c>
+      <c r="D333">
+        <v>3</v>
+      </c>
+      <c r="E333" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>332</v>
       </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B334" t="s">
+        <v>380</v>
+      </c>
+      <c r="C334">
+        <v>3</v>
+      </c>
+      <c r="D334">
+        <v>3</v>
+      </c>
+      <c r="E334" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>333</v>
       </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B335" t="s">
+        <v>361</v>
+      </c>
+      <c r="C335">
+        <v>3</v>
+      </c>
+      <c r="D335">
+        <v>3</v>
+      </c>
+      <c r="E335" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>334</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B336" t="s">
+        <v>362</v>
+      </c>
+      <c r="C336">
+        <v>1</v>
+      </c>
+      <c r="D336">
+        <v>3</v>
+      </c>
+      <c r="E336" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>335</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B337" t="s">
+        <v>363</v>
+      </c>
+      <c r="C337">
+        <v>3</v>
+      </c>
+      <c r="D337">
+        <v>3</v>
+      </c>
+      <c r="E337" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>336</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B338" t="s">
+        <v>364</v>
+      </c>
+      <c r="C338">
+        <v>1</v>
+      </c>
+      <c r="D338">
+        <v>3</v>
+      </c>
+      <c r="E338" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>337</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B339" t="s">
+        <v>365</v>
+      </c>
+      <c r="C339">
+        <v>1</v>
+      </c>
+      <c r="D339">
+        <v>3</v>
+      </c>
+      <c r="E339" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>338</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B340" t="s">
+        <v>366</v>
+      </c>
+      <c r="C340">
+        <v>1</v>
+      </c>
+      <c r="D340">
+        <v>3</v>
+      </c>
+      <c r="E340" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>339</v>
+      </c>
+      <c r="B341" t="s">
+        <v>367</v>
+      </c>
+      <c r="C341">
+        <v>1</v>
+      </c>
+      <c r="D341">
+        <v>2</v>
+      </c>
+      <c r="E341" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>340</v>
+      </c>
+      <c r="B342" t="s">
+        <v>368</v>
+      </c>
+      <c r="C342">
+        <v>1</v>
+      </c>
+      <c r="D342">
+        <v>2</v>
+      </c>
+      <c r="E342" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>341</v>
+      </c>
+      <c r="B343" t="s">
+        <v>369</v>
+      </c>
+      <c r="C343">
+        <v>1</v>
+      </c>
+      <c r="D343">
+        <v>2</v>
+      </c>
+      <c r="E343" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>342</v>
+      </c>
+      <c r="B344" t="s">
+        <v>370</v>
+      </c>
+      <c r="C344">
+        <v>1</v>
+      </c>
+      <c r="D344">
+        <v>2</v>
+      </c>
+      <c r="E344" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>343</v>
+      </c>
+      <c r="B345" t="s">
+        <v>371</v>
+      </c>
+      <c r="C345">
+        <v>1</v>
+      </c>
+      <c r="D345">
+        <v>2</v>
+      </c>
+      <c r="E345" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>344</v>
+      </c>
+      <c r="B346" t="s">
+        <v>372</v>
+      </c>
+      <c r="C346">
+        <v>1</v>
+      </c>
+      <c r="D346">
+        <v>2</v>
+      </c>
+      <c r="E346" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>345</v>
+      </c>
+      <c r="B347" t="s">
+        <v>373</v>
+      </c>
+      <c r="C347">
+        <v>1</v>
+      </c>
+      <c r="D347">
+        <v>2</v>
+      </c>
+      <c r="E347" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>346</v>
+      </c>
+      <c r="B348" t="s">
+        <v>374</v>
+      </c>
+      <c r="C348">
+        <v>1</v>
+      </c>
+      <c r="D348">
+        <v>2</v>
+      </c>
+      <c r="E348" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>347</v>
+      </c>
+      <c r="B349" t="s">
+        <v>375</v>
+      </c>
+      <c r="C349">
+        <v>1</v>
+      </c>
+      <c r="D349">
+        <v>2</v>
+      </c>
+      <c r="E349" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>348</v>
+      </c>
+      <c r="B350" t="s">
+        <v>376</v>
+      </c>
+      <c r="C350">
+        <v>1</v>
+      </c>
+      <c r="D350">
+        <v>2</v>
+      </c>
+      <c r="E350" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>349</v>
+      </c>
+      <c r="B351" t="s">
+        <v>377</v>
+      </c>
+      <c r="C351">
+        <v>1</v>
+      </c>
+      <c r="D351">
+        <v>2</v>
+      </c>
+      <c r="E351" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>350</v>
+      </c>
+      <c r="B352" t="s">
+        <v>378</v>
+      </c>
+      <c r="C352">
+        <v>1</v>
+      </c>
+      <c r="D352">
+        <v>1</v>
+      </c>
+      <c r="E352" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>